<commit_message>
informe de comunas ok
</commit_message>
<xml_diff>
--- a/InformePorComuna.xlsx
+++ b/InformePorComuna.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Comuna</t>
   </si>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>$20000</t>
+  </si>
+  <si>
+    <t>Total Cantidad</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Total precio</t>
+  </si>
+  <si>
+    <t>$70000</t>
   </si>
 </sst>
 </file>
@@ -89,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -137,6 +149,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>